<commit_message>
remove preprocess image ocr
</commit_message>
<xml_diff>
--- a/vehicle_data.xlsx
+++ b/vehicle_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,6 +455,126 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>77A-247.01</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Top</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-11-02 12:55:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>77A-247.01</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Top</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-11-02 14:11:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>CN4</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Bottom</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-11-02 14:21:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>322</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Bottom</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2025-11-02 14:25:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>77C-226.75</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Bottom</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2025-11-02 14:56:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>35</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>77A-247.01</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Top</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2025-11-02 14:56:45</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
split file to modules
</commit_message>
<xml_diff>
--- a/vehicle_data.xlsx
+++ b/vehicle_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -575,6 +575,126 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>77C-226.75</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Bottom</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2025-11-02 18:25:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>35</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>77A-247.01</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Top</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2025-11-02 18:25:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>77C-226.75</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Bottom</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2025-11-18 22:40:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>35</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>77A-247.01</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Top</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2025-11-18 22:40:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>77C-226.75</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Bottom</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2025-11-18 22:51:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>35</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>77A-247.01</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Top</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2025-11-18 22:51:48</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
add: send mess for telegram bot
</commit_message>
<xml_diff>
--- a/vehicle_data.xlsx
+++ b/vehicle_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -695,6 +695,66 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>77C-226.75</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Bottom</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2025-11-22 22:49:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>77C-226.75</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Bottom</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2025-11-22 23:40:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>35</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>77A-247.01</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Top</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2025-11-22 23:40:31</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: send duplicate mess telegram
</commit_message>
<xml_diff>
--- a/vehicle_data.xlsx
+++ b/vehicle_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -755,6 +755,46 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>1</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>77C-226.75</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Bottom</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2025-11-25 23:08:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>35</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>77A-247.01</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Top</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2025-11-25 23:09:01</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
add: condition for check lp
</commit_message>
<xml_diff>
--- a/vehicle_data.xlsx
+++ b/vehicle_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -795,6 +795,146 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>77H052.79</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Bottom</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2025-11-27 23:16:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>12</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>GLZ50RLL</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Bottom</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2025-11-27 23:16:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>77H052.79</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Bottom</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2025-11-27 23:42:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>12</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>177806279</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Bottom</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>2025-11-27 23:42:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>1</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>77H052.79</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Bottom</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>2025-11-27 23:47:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>12</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>77H052.79</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Bottom</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>2025-11-27 23:47:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>1</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>77H-052.79</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Bottom</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>2025-11-27 23:55:10</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>